<commit_message>
backup trước khi thay đổi csdl cho chức năng hiển thị nhiều năm.
</commit_message>
<xml_diff>
--- a/Docs/Report/Tính giá trị phần mềm web hỗ trợ tuyển sinh.xlsx
+++ b/Docs/Report/Tính giá trị phần mềm web hỗ trợ tuyển sinh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Giá trị phần mềm" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="243">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -813,17 +813,21 @@
   <si>
     <t>NV tuyển sinh</t>
   </si>
+  <si>
+    <t>Hiển thị cờ theo năm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$VND]"/>
     <numFmt numFmtId="166" formatCode="#,##0\ [$VND/người/giờ]"/>
     <numFmt numFmtId="167" formatCode="0.00\ [$giờ]"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="#,##0\ [$VND]"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -1661,7 +1665,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1999,27 +2003,87 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2062,54 +2126,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2152,18 +2168,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2176,12 +2198,6 @@
     <xf numFmtId="2" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2218,16 +2234,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2689,7 +2714,7 @@
         <xdr:cNvPr id="6" name="Picture 5" descr="Abstract Image" title="Banner 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63FC21FF-CA95-46EB-A920-3C0D718BE000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63FC21FF-CA95-46EB-A920-3C0D718BE000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2739,7 +2764,7 @@
         <xdr:cNvPr id="8" name="TextBox 1" descr="Sales Receipt" title="Title 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1AC2A7CC-8F12-414F-B76E-CBE4CCE99AAC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AC2A7CC-8F12-414F-B76E-CBE4CCE99AAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2824,7 +2849,7 @@
         <xdr:cNvPr id="9" name="TextBox 8" descr="Company Slogan" title="Title 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EFAF2BFD-D500-4AA7-9B34-C8624A8E9FD9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAF2BFD-D500-4AA7-9B34-C8624A8E9FD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2903,7 +2928,7 @@
         <xdr:cNvPr id="10" name="TextBox 2" descr="Company Name" title="Title 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6734F8B5-6D8A-4FF7-91D7-88784131B17C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6734F8B5-6D8A-4FF7-91D7-88784131B17C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3241,8 +3266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -3270,10 +3295,10 @@
       <c r="D2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="122"/>
+      <c r="F2" s="142"/>
     </row>
     <row r="3" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="B3" s="1" t="s">
@@ -3282,10 +3307,10 @@
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="123">
+      <c r="E3" s="143">
         <v>43413</v>
       </c>
-      <c r="F3" s="123"/>
+      <c r="F3" s="143"/>
     </row>
     <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="12" t="s">
@@ -3297,11 +3322,11 @@
       <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="9" spans="1:8" ht="30" customHeight="1">
@@ -3314,11 +3339,11 @@
       <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="117" t="s">
+      <c r="D9" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
     </row>
     <row r="10" spans="1:8" ht="45.75" customHeight="1">
       <c r="A10" s="14" t="s">
@@ -3330,12 +3355,12 @@
       <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="119">
+      <c r="D10" s="117">
         <f>E</f>
-        <v>141.42333333333335</v>
-      </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="121"/>
+        <v>167.50824999999998</v>
+      </c>
+      <c r="E10" s="118"/>
+      <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:8" ht="45.75" customHeight="1">
       <c r="A11" s="15" t="s">
@@ -3347,12 +3372,12 @@
       <c r="C11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="124">
+      <c r="D11" s="144">
         <f>'Phụlục VI-2'!F17</f>
         <v>20</v>
       </c>
-      <c r="E11" s="125"/>
-      <c r="F11" s="126"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="146"/>
     </row>
     <row r="12" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
       <c r="A12" s="15" t="s">
@@ -3364,30 +3389,30 @@
       <c r="C12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="127">
-        <v>20</v>
-      </c>
-      <c r="E12" s="128"/>
-      <c r="F12" s="129"/>
+      <c r="D12" s="147">
+        <v>20000</v>
+      </c>
+      <c r="E12" s="148"/>
+      <c r="F12" s="149"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="137"/>
-      <c r="E13" s="137"/>
-      <c r="F13" s="137"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1">
       <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="130">
+      <c r="D14" s="195">
         <f xml:space="preserve"> 1.4 * D10 * D11 * D12 * 1.1</f>
-        <v>87116.773333333345</v>
-      </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+        <v>103185081.99999997</v>
+      </c>
+      <c r="E14" s="196"/>
+      <c r="F14" s="197"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
       <c r="A15" s="9" t="s">
@@ -3396,14 +3421,14 @@
       <c r="C15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="130">
+      <c r="D15" s="150">
         <v>0</v>
       </c>
-      <c r="E15" s="131" t="e">
+      <c r="E15" s="151" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="F15" s="132"/>
+      <c r="F15" s="152"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="24" customHeight="1">
@@ -3413,25 +3438,25 @@
       <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="133">
+      <c r="D16" s="153">
         <v>0</v>
       </c>
-      <c r="E16" s="134">
+      <c r="E16" s="154">
         <v>0</v>
       </c>
-      <c r="F16" s="135"/>
+      <c r="F16" s="155"/>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="24" customHeight="1">
       <c r="C17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="136">
+      <c r="D17" s="198">
         <f>(D14+D15)*(1-D16)</f>
-        <v>87116.773333333345</v>
-      </c>
-      <c r="E17" s="136"/>
-      <c r="F17" s="136"/>
+        <v>103185081.99999997</v>
+      </c>
+      <c r="E17" s="198"/>
+      <c r="F17" s="198"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8"/>
@@ -3445,11 +3470,11 @@
       <c r="F19" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B21" s="115" t="s">
+      <c r="B21" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="116"/>
-      <c r="D21" s="116"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="23" spans="1:6" ht="30" customHeight="1">
@@ -3462,11 +3487,11 @@
       <c r="C23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="117" t="s">
+      <c r="D23" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
     </row>
     <row r="24" spans="1:6" ht="45.75" customHeight="1" thickBot="1">
       <c r="A24" s="15" t="s">
@@ -3478,31 +3503,31 @@
       <c r="C24" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="119">
+      <c r="D24" s="117">
         <f>AUCP</f>
-        <v>84.853999999999999</v>
-      </c>
-      <c r="E24" s="120"/>
-      <c r="F24" s="121"/>
+        <v>100.50494999999998</v>
+      </c>
+      <c r="E24" s="118"/>
+      <c r="F24" s="119"/>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="137"/>
-      <c r="F25" s="137"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="120"/>
     </row>
     <row r="26" spans="1:6" ht="24" customHeight="1" thickBot="1">
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="147">
+      <c r="D26" s="121">
         <f>10 / 6 * D24</f>
-        <v>141.42333333333335</v>
-      </c>
-      <c r="E26" s="148"/>
-      <c r="F26" s="149"/>
+        <v>167.50824999999998</v>
+      </c>
+      <c r="E26" s="122"/>
+      <c r="F26" s="123"/>
     </row>
     <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3533,11 +3558,11 @@
       <c r="C32" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="117" t="s">
+      <c r="D32" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="118"/>
-      <c r="F32" s="118"/>
+      <c r="E32" s="130"/>
+      <c r="F32" s="130"/>
     </row>
     <row r="33" spans="1:7" ht="45.75" customHeight="1">
       <c r="A33" s="15" t="s">
@@ -3547,12 +3572,12 @@
         <v>33</v>
       </c>
       <c r="C33" s="16"/>
-      <c r="D33" s="119">
+      <c r="D33" s="117">
         <f>UUCP</f>
-        <v>116</v>
-      </c>
-      <c r="E33" s="120"/>
-      <c r="F33" s="121"/>
+        <v>111</v>
+      </c>
+      <c r="E33" s="118"/>
+      <c r="F33" s="119"/>
     </row>
     <row r="34" spans="1:7" ht="45.75" customHeight="1">
       <c r="A34" s="15" t="s">
@@ -3562,12 +3587,12 @@
         <v>34</v>
       </c>
       <c r="C34" s="16"/>
-      <c r="D34" s="138">
+      <c r="D34" s="137">
         <f>TCF</f>
-        <v>0.77</v>
-      </c>
-      <c r="E34" s="139"/>
-      <c r="F34" s="140"/>
+        <v>0.90999999999999992</v>
+      </c>
+      <c r="E34" s="138"/>
+      <c r="F34" s="139"/>
     </row>
     <row r="35" spans="1:7" ht="45.75" customHeight="1" thickBot="1">
       <c r="A35" s="15" t="s">
@@ -3577,31 +3602,31 @@
         <v>35</v>
       </c>
       <c r="C35" s="16"/>
-      <c r="D35" s="144">
+      <c r="D35" s="134">
         <f>EF</f>
-        <v>0.95</v>
-      </c>
-      <c r="E35" s="145"/>
-      <c r="F35" s="146"/>
+        <v>0.99499999999999988</v>
+      </c>
+      <c r="E35" s="135"/>
+      <c r="F35" s="136"/>
     </row>
     <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="137"/>
-      <c r="E36" s="137"/>
-      <c r="F36" s="137"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
     </row>
     <row r="37" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="C37" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="147">
+      <c r="D37" s="121">
         <f xml:space="preserve"> D33 * D34 * D35</f>
-        <v>84.853999999999999</v>
-      </c>
-      <c r="E37" s="148"/>
-      <c r="F37" s="149"/>
+        <v>100.50494999999998</v>
+      </c>
+      <c r="E37" s="122"/>
+      <c r="F37" s="123"/>
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3632,11 +3657,11 @@
       <c r="C43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="117" t="s">
+      <c r="D43" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118"/>
+      <c r="E43" s="130"/>
+      <c r="F43" s="130"/>
     </row>
     <row r="44" spans="1:7" ht="45.75" customHeight="1">
       <c r="A44" s="15" t="s">
@@ -3648,12 +3673,12 @@
       <c r="C44" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="119">
+      <c r="D44" s="117">
         <f>'Phụ lục III'!E8</f>
         <v>6</v>
       </c>
-      <c r="E44" s="120"/>
-      <c r="F44" s="121"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="119"/>
       <c r="G44" s="1" t="s">
         <v>69</v>
       </c>
@@ -3668,12 +3693,12 @@
       <c r="C45" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="141">
+      <c r="D45" s="131">
         <f>'Phụ lục IV'!D17:F17</f>
-        <v>110</v>
-      </c>
-      <c r="E45" s="142"/>
-      <c r="F45" s="143"/>
+        <v>105</v>
+      </c>
+      <c r="E45" s="132"/>
+      <c r="F45" s="133"/>
       <c r="G45" s="1" t="s">
         <v>70</v>
       </c>
@@ -3682,20 +3707,20 @@
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="137"/>
-      <c r="E46" s="137"/>
-      <c r="F46" s="137"/>
+      <c r="D46" s="120"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="120"/>
     </row>
     <row r="47" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="C47" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="147">
+      <c r="D47" s="121">
         <f xml:space="preserve"> D44 + D45</f>
-        <v>116</v>
-      </c>
-      <c r="E47" s="148"/>
-      <c r="F47" s="149"/>
+        <v>111</v>
+      </c>
+      <c r="E47" s="122"/>
+      <c r="F47" s="123"/>
     </row>
     <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3707,13 +3732,13 @@
       <c r="F49" s="17"/>
     </row>
     <row r="51" spans="1:7" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B51" s="150" t="s">
+      <c r="B51" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="151"/>
-      <c r="D51" s="151"/>
-      <c r="E51" s="151"/>
-      <c r="F51" s="151"/>
+      <c r="C51" s="128"/>
+      <c r="D51" s="128"/>
+      <c r="E51" s="128"/>
+      <c r="F51" s="128"/>
     </row>
     <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="53" spans="1:7" ht="30" customHeight="1">
@@ -3726,11 +3751,11 @@
       <c r="C53" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="117" t="s">
+      <c r="D53" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
+      <c r="E53" s="130"/>
+      <c r="F53" s="130"/>
     </row>
     <row r="54" spans="1:7" ht="45.75" customHeight="1" thickBot="1">
       <c r="A54" s="15" t="s">
@@ -3742,12 +3767,12 @@
       <c r="C54" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="119">
+      <c r="D54" s="117">
         <f>'Phụ lục V'!E5</f>
-        <v>17</v>
-      </c>
-      <c r="E54" s="120"/>
-      <c r="F54" s="121"/>
+        <v>31</v>
+      </c>
+      <c r="E54" s="118"/>
+      <c r="F54" s="119"/>
       <c r="G54" s="1" t="s">
         <v>117</v>
       </c>
@@ -3756,20 +3781,20 @@
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="137"/>
-      <c r="E55" s="137"/>
-      <c r="F55" s="137"/>
+      <c r="D55" s="120"/>
+      <c r="E55" s="120"/>
+      <c r="F55" s="120"/>
     </row>
     <row r="56" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="C56" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D56" s="189">
+      <c r="D56" s="124">
         <f>0.6 + (0.01 * D54)</f>
-        <v>0.77</v>
-      </c>
-      <c r="E56" s="190"/>
-      <c r="F56" s="191"/>
+        <v>0.90999999999999992</v>
+      </c>
+      <c r="E56" s="125"/>
+      <c r="F56" s="126"/>
     </row>
     <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3781,13 +3806,13 @@
       <c r="F58" s="17"/>
     </row>
     <row r="60" spans="1:7" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B60" s="150" t="s">
+      <c r="B60" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="151"/>
-      <c r="D60" s="151"/>
-      <c r="E60" s="151"/>
-      <c r="F60" s="151"/>
+      <c r="C60" s="128"/>
+      <c r="D60" s="128"/>
+      <c r="E60" s="128"/>
+      <c r="F60" s="128"/>
     </row>
     <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="62" spans="1:7" ht="30" customHeight="1">
@@ -3800,11 +3825,11 @@
       <c r="C62" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="117" t="s">
+      <c r="D62" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="118"/>
-      <c r="F62" s="118"/>
+      <c r="E62" s="130"/>
+      <c r="F62" s="130"/>
     </row>
     <row r="63" spans="1:7" ht="45.75" customHeight="1" thickBot="1">
       <c r="A63" s="15" t="s">
@@ -3816,12 +3841,12 @@
       <c r="C63" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D63" s="119">
+      <c r="D63" s="117">
         <f>'Phụlục VI-2'!E5</f>
-        <v>15</v>
-      </c>
-      <c r="E63" s="120"/>
-      <c r="F63" s="121"/>
+        <v>13.5</v>
+      </c>
+      <c r="E63" s="118"/>
+      <c r="F63" s="119"/>
       <c r="G63" s="1" t="s">
         <v>218</v>
       </c>
@@ -3830,47 +3855,24 @@
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="137"/>
-      <c r="E64" s="137"/>
-      <c r="F64" s="137"/>
+      <c r="D64" s="120"/>
+      <c r="E64" s="120"/>
+      <c r="F64" s="120"/>
     </row>
     <row r="65" spans="3:6" ht="24" customHeight="1" thickBot="1">
       <c r="C65" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D65" s="147">
+      <c r="D65" s="121">
         <f>1.4 + (-0.03 * D63)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E65" s="148"/>
-      <c r="F65" s="149"/>
+        <v>0.99499999999999988</v>
+      </c>
+      <c r="E65" s="122"/>
+      <c r="F65" s="123"/>
     </row>
     <row r="66" spans="3:6" ht="20.100000000000001" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="D23:F23"/>
@@ -3886,6 +3888,29 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Customer Information to the right section" sqref="A2"/>
@@ -3935,8 +3960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3974,11 +3999,11 @@
       <c r="C4" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="152" t="s">
+      <c r="D4" s="156" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
     </row>
     <row r="5" spans="1:12" ht="39.75" customHeight="1">
       <c r="A5" s="39">
@@ -3986,9 +4011,9 @@
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="29"/>
-      <c r="D5" s="153"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="155"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="159"/>
     </row>
     <row r="6" spans="1:12" ht="39.75" customHeight="1">
       <c r="A6" s="39">
@@ -4136,9 +4161,9 @@
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="29"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="161"/>
+      <c r="F20" s="162"/>
     </row>
     <row r="21" spans="1:6" ht="39.75" customHeight="1">
       <c r="A21" s="39">
@@ -4146,9 +4171,9 @@
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="29"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="160"/>
-      <c r="F21" s="161"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="164"/>
+      <c r="F21" s="165"/>
     </row>
     <row r="22" spans="1:6" ht="39.75" customHeight="1" thickBot="1">
       <c r="A22" s="40">
@@ -4156,9 +4181,9 @@
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="32"/>
-      <c r="D22" s="162"/>
-      <c r="E22" s="163"/>
-      <c r="F22" s="164"/>
+      <c r="D22" s="166"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="168"/>
     </row>
     <row r="23" spans="1:6" ht="15" thickTop="1"/>
     <row r="24" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -4185,10 +4210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G26"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G25" sqref="G5:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4201,13 +4226,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="169" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickTop="1">
       <c r="A3" s="38"/>
@@ -4404,7 +4429,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="C14" s="62" t="s">
         <v>240</v>
@@ -4421,7 +4446,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="62" t="s">
         <v>240</v>
@@ -4438,7 +4463,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>240</v>
@@ -4455,7 +4480,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C17" s="62" t="s">
         <v>240</v>
@@ -4472,10 +4497,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C18" s="62" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D18" s="102"/>
       <c r="E18" s="102"/>
@@ -4489,7 +4514,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C19" s="62" t="s">
         <v>239</v>
@@ -4506,23 +4531,24 @@
         <v>16</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C20" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="D20" s="104"/>
-      <c r="E20" s="105"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
       <c r="F20" s="109" t="s">
         <v>89</v>
       </c>
+      <c r="G20" s="103"/>
     </row>
     <row r="21" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
       <c r="A21" s="57">
         <v>17</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>239</v>
@@ -4532,13 +4558,14 @@
       <c r="F21" s="109" t="s">
         <v>89</v>
       </c>
+      <c r="G21" s="192"/>
     </row>
     <row r="22" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
       <c r="A22" s="57">
         <v>18</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C22" s="62" t="s">
         <v>239</v>
@@ -4548,47 +4575,67 @@
       <c r="F22" s="109" t="s">
         <v>89</v>
       </c>
+      <c r="G22" s="192"/>
     </row>
     <row r="23" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
       <c r="A23" s="57">
         <v>19</v>
       </c>
-      <c r="B23" s="112" t="s">
-        <v>237</v>
+      <c r="B23" s="58" t="s">
+        <v>236</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="105"/>
       <c r="F23" s="109" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A24" s="40">
+      <c r="G23" s="192"/>
+    </row>
+    <row r="24" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A24" s="57">
         <v>20</v>
       </c>
-      <c r="B24" s="60" t="s">
-        <v>238</v>
-      </c>
-      <c r="C24" s="106" t="s">
+      <c r="B24" s="112" t="s">
+        <v>237</v>
+      </c>
+      <c r="C24" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="D24" s="106"/>
-      <c r="E24" s="107"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="113"/>
       <c r="F24" s="109" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickTop="1"/>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="108"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="110"/>
+      <c r="G24" s="192"/>
+    </row>
+    <row r="25" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
+      <c r="A25" s="60">
+        <v>21</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="106" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" s="106"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="115" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="192"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickTop="1"/>
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A27" s="17"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4604,7 +4651,7 @@
   <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4620,13 +4667,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="48.75" customHeight="1" thickBot="1">
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="169" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1">
       <c r="A3" s="38"/>
@@ -4787,7 +4834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -4804,18 +4851,18 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="47.25" customHeight="1" thickBot="1">
       <c r="A2" s="22"/>
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="169" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
+      <c r="I2" s="175"/>
+      <c r="J2" s="175"/>
+      <c r="K2" s="175"/>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickTop="1"/>
@@ -4829,11 +4876,11 @@
       <c r="C4" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="170" t="s">
+      <c r="D4" s="176" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
       <c r="H4" s="23" t="s">
         <v>58</v>
       </c>
@@ -4855,12 +4902,12 @@
         <v>89</v>
       </c>
       <c r="C5" s="69"/>
-      <c r="D5" s="171">
+      <c r="D5" s="177">
         <f>SUM(D6:F8)</f>
-        <v>110</v>
-      </c>
-      <c r="E5" s="172"/>
-      <c r="F5" s="173"/>
+        <v>105</v>
+      </c>
+      <c r="E5" s="178"/>
+      <c r="F5" s="179"/>
       <c r="H5" s="57">
         <v>1</v>
       </c>
@@ -4876,14 +4923,14 @@
         <v>90</v>
       </c>
       <c r="C6" s="47">
-        <v>18</v>
-      </c>
-      <c r="D6" s="153">
+        <v>21</v>
+      </c>
+      <c r="D6" s="157">
         <f>C6 * J6 * K6</f>
-        <v>90</v>
-      </c>
-      <c r="E6" s="154"/>
-      <c r="F6" s="155"/>
+        <v>105</v>
+      </c>
+      <c r="E6" s="158"/>
+      <c r="F6" s="159"/>
       <c r="H6" s="57"/>
       <c r="I6" s="62" t="s">
         <v>90</v>
@@ -4901,14 +4948,14 @@
         <v>91</v>
       </c>
       <c r="C7" s="47">
-        <v>2</v>
-      </c>
-      <c r="D7" s="153">
+        <v>0</v>
+      </c>
+      <c r="D7" s="157">
         <f>C7 * J7 * K7</f>
-        <v>20</v>
-      </c>
-      <c r="E7" s="154"/>
-      <c r="F7" s="155"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="158"/>
+      <c r="F7" s="159"/>
       <c r="H7" s="57"/>
       <c r="I7" s="62" t="s">
         <v>91</v>
@@ -4928,12 +4975,12 @@
       <c r="C8" s="47">
         <v>0</v>
       </c>
-      <c r="D8" s="153">
+      <c r="D8" s="157">
         <f>C8 * J8 * K8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="154"/>
-      <c r="F8" s="155"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="159"/>
       <c r="H8" s="57"/>
       <c r="I8" s="62" t="s">
         <v>92</v>
@@ -4953,12 +5000,12 @@
         <v>93</v>
       </c>
       <c r="C9" s="69"/>
-      <c r="D9" s="167">
+      <c r="D9" s="172">
         <f>SUM(D10:F12)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="168"/>
-      <c r="F9" s="169"/>
+      <c r="E9" s="173"/>
+      <c r="F9" s="174"/>
       <c r="H9" s="57">
         <v>2</v>
       </c>
@@ -4976,12 +5023,12 @@
       <c r="C10" s="47">
         <v>0</v>
       </c>
-      <c r="D10" s="153">
+      <c r="D10" s="157">
         <f>C10 * J10 * K10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="154"/>
-      <c r="F10" s="155"/>
+      <c r="E10" s="158"/>
+      <c r="F10" s="159"/>
       <c r="H10" s="57"/>
       <c r="I10" s="62" t="s">
         <v>90</v>
@@ -5001,12 +5048,12 @@
       <c r="C11" s="47">
         <v>0</v>
       </c>
-      <c r="D11" s="153">
+      <c r="D11" s="157">
         <f>C11 * J11 * K11</f>
         <v>0</v>
       </c>
-      <c r="E11" s="154"/>
-      <c r="F11" s="155"/>
+      <c r="E11" s="158"/>
+      <c r="F11" s="159"/>
       <c r="H11" s="57"/>
       <c r="I11" s="62" t="s">
         <v>91</v>
@@ -5026,12 +5073,12 @@
       <c r="C12" s="47">
         <v>0</v>
       </c>
-      <c r="D12" s="153">
+      <c r="D12" s="157">
         <f>C12 * J12 * K12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="154"/>
-      <c r="F12" s="155"/>
+      <c r="E12" s="158"/>
+      <c r="F12" s="159"/>
       <c r="H12" s="57"/>
       <c r="I12" s="62" t="s">
         <v>92</v>
@@ -5051,12 +5098,12 @@
         <v>94</v>
       </c>
       <c r="C13" s="69"/>
-      <c r="D13" s="167">
+      <c r="D13" s="172">
         <f>SUM(D14:F16)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="168"/>
-      <c r="F13" s="169"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="174"/>
       <c r="H13" s="57">
         <v>3</v>
       </c>
@@ -5074,12 +5121,12 @@
       <c r="C14" s="47">
         <v>0</v>
       </c>
-      <c r="D14" s="153">
+      <c r="D14" s="157">
         <f>C14 * J14 * K14</f>
         <v>0</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="155"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="159"/>
       <c r="H14" s="57"/>
       <c r="I14" s="62" t="s">
         <v>90</v>
@@ -5099,12 +5146,12 @@
       <c r="C15" s="47">
         <v>0</v>
       </c>
-      <c r="D15" s="153">
+      <c r="D15" s="157">
         <f>C15 * J15 * K15</f>
         <v>0</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="155"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="159"/>
       <c r="H15" s="57"/>
       <c r="I15" s="62" t="s">
         <v>91</v>
@@ -5124,12 +5171,12 @@
       <c r="C16" s="47">
         <v>0</v>
       </c>
-      <c r="D16" s="153">
+      <c r="D16" s="157">
         <f>C16 * J16 * K16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="155"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="159"/>
       <c r="H16" s="59"/>
       <c r="I16" s="63" t="s">
         <v>92</v>
@@ -5151,12 +5198,12 @@
       <c r="C17" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="174">
+      <c r="D17" s="170">
         <f xml:space="preserve"> D5 + D9 + D13</f>
-        <v>110</v>
-      </c>
-      <c r="E17" s="145"/>
-      <c r="F17" s="175"/>
+        <v>105</v>
+      </c>
+      <c r="E17" s="135"/>
+      <c r="F17" s="171"/>
     </row>
     <row r="18" spans="1:11" ht="15" thickTop="1"/>
     <row r="19" spans="1:11" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -5175,11 +5222,6 @@
     <row r="20" spans="1:11" s="1" customFormat="1" ht="20.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D10:F10"/>
@@ -5190,6 +5232,11 @@
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5199,8 +5246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5216,13 +5263,13 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A2" s="22"/>
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="169" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -5264,9 +5311,9 @@
       </c>
       <c r="C5" s="64"/>
       <c r="D5" s="43"/>
-      <c r="E5" s="188">
+      <c r="E5" s="116">
         <f xml:space="preserve"> SUM(E6:E18)</f>
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F5" s="74"/>
     </row>
@@ -5281,11 +5328,11 @@
         <v>2</v>
       </c>
       <c r="D6" s="43">
-        <v>0</v>
-      </c>
-      <c r="E6" s="188">
-        <f>D6 * C6</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E6" s="116">
+        <f t="shared" ref="E6:E18" si="0">D6 * C6</f>
+        <v>4</v>
       </c>
       <c r="F6" s="74"/>
     </row>
@@ -5300,11 +5347,11 @@
         <v>1</v>
       </c>
       <c r="D7" s="43">
-        <v>0</v>
-      </c>
-      <c r="E7" s="188">
-        <f>D7 * C7</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E7" s="116">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F7" s="74"/>
     </row>
@@ -5321,8 +5368,8 @@
       <c r="D8" s="43">
         <v>1</v>
       </c>
-      <c r="E8" s="188">
-        <f>D8 * C8</f>
+      <c r="E8" s="116">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F8" s="74"/>
@@ -5338,11 +5385,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="43">
-        <v>2</v>
-      </c>
-      <c r="E9" s="188">
-        <f>D9 * C9</f>
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E9" s="116">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="F9" s="74"/>
     </row>
@@ -5357,11 +5404,11 @@
         <v>1</v>
       </c>
       <c r="D10" s="43">
-        <v>0</v>
-      </c>
-      <c r="E10" s="188">
-        <f>D10 * C10</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E10" s="116">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="F10" s="74"/>
     </row>
@@ -5376,11 +5423,11 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="43">
-        <v>0</v>
-      </c>
-      <c r="E11" s="188">
-        <f>D11 * C11</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E11" s="116">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="F11" s="74"/>
     </row>
@@ -5395,11 +5442,11 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="43">
-        <v>0</v>
-      </c>
-      <c r="E12" s="188">
-        <f>D12 * C12</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E12" s="116">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="F12" s="74"/>
     </row>
@@ -5414,11 +5461,11 @@
         <v>2</v>
       </c>
       <c r="D13" s="43">
-        <v>1</v>
-      </c>
-      <c r="E13" s="188">
-        <f>D13 * C13</f>
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E13" s="116">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="F13" s="74"/>
     </row>
@@ -5435,8 +5482,8 @@
       <c r="D14" s="43">
         <v>3</v>
       </c>
-      <c r="E14" s="188">
-        <f>D14 * C14</f>
+      <c r="E14" s="116">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F14" s="74"/>
@@ -5452,11 +5499,11 @@
         <v>1</v>
       </c>
       <c r="D15" s="43">
-        <v>2</v>
-      </c>
-      <c r="E15" s="188">
-        <f>D15 * C15</f>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E15" s="116">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F15" s="74"/>
     </row>
@@ -5473,8 +5520,8 @@
       <c r="D16" s="43">
         <v>2</v>
       </c>
-      <c r="E16" s="188">
-        <f>D16 * C16</f>
+      <c r="E16" s="116">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F16" s="74"/>
@@ -5490,11 +5537,11 @@
         <v>1</v>
       </c>
       <c r="D17" s="43">
-        <v>4</v>
-      </c>
-      <c r="E17" s="188">
-        <f>D17 * C17</f>
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E17" s="116">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="F17" s="74"/>
     </row>
@@ -5512,7 +5559,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="114">
-        <f>D18 * C18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F18" s="82"/>
@@ -5539,17 +5586,17 @@
       <c r="B22" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="182" t="s">
+      <c r="C22" s="186" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="183"/>
-      <c r="E22" s="183"/>
-      <c r="F22" s="183"/>
-      <c r="G22" s="183"/>
-      <c r="H22" s="183"/>
-      <c r="I22" s="183"/>
-      <c r="J22" s="183"/>
-      <c r="K22" s="183"/>
+      <c r="D22" s="187"/>
+      <c r="E22" s="187"/>
+      <c r="F22" s="187"/>
+      <c r="G22" s="187"/>
+      <c r="H22" s="187"/>
+      <c r="I22" s="187"/>
+      <c r="J22" s="187"/>
+      <c r="K22" s="187"/>
     </row>
     <row r="23" spans="1:11" ht="99.75" customHeight="1">
       <c r="A23" s="76">
@@ -5558,17 +5605,17 @@
       <c r="B23" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="176" t="s">
+      <c r="C23" s="180" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="177"/>
-      <c r="E23" s="177"/>
-      <c r="F23" s="177"/>
-      <c r="G23" s="177"/>
-      <c r="H23" s="177"/>
-      <c r="I23" s="177"/>
-      <c r="J23" s="177"/>
-      <c r="K23" s="178"/>
+      <c r="D23" s="181"/>
+      <c r="E23" s="181"/>
+      <c r="F23" s="181"/>
+      <c r="G23" s="181"/>
+      <c r="H23" s="181"/>
+      <c r="I23" s="181"/>
+      <c r="J23" s="181"/>
+      <c r="K23" s="182"/>
     </row>
     <row r="24" spans="1:11" ht="142.5" customHeight="1">
       <c r="A24" s="76">
@@ -5577,17 +5624,17 @@
       <c r="B24" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="176" t="s">
+      <c r="C24" s="180" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="177"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="177"/>
-      <c r="G24" s="177"/>
-      <c r="H24" s="177"/>
-      <c r="I24" s="177"/>
-      <c r="J24" s="177"/>
-      <c r="K24" s="178"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="181"/>
+      <c r="K24" s="182"/>
     </row>
     <row r="25" spans="1:11" ht="99.75" customHeight="1">
       <c r="A25" s="76">
@@ -5596,17 +5643,17 @@
       <c r="B25" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="176" t="s">
+      <c r="C25" s="180" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="177"/>
-      <c r="E25" s="177"/>
-      <c r="F25" s="177"/>
-      <c r="G25" s="177"/>
-      <c r="H25" s="177"/>
-      <c r="I25" s="177"/>
-      <c r="J25" s="177"/>
-      <c r="K25" s="178"/>
+      <c r="D25" s="181"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="181"/>
+      <c r="G25" s="181"/>
+      <c r="H25" s="181"/>
+      <c r="I25" s="181"/>
+      <c r="J25" s="181"/>
+      <c r="K25" s="182"/>
     </row>
     <row r="26" spans="1:11" ht="142.5" customHeight="1">
       <c r="A26" s="76">
@@ -5615,17 +5662,17 @@
       <c r="B26" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="176" t="s">
+      <c r="C26" s="180" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="177"/>
-      <c r="E26" s="177"/>
-      <c r="F26" s="177"/>
-      <c r="G26" s="177"/>
-      <c r="H26" s="177"/>
-      <c r="I26" s="177"/>
-      <c r="J26" s="177"/>
-      <c r="K26" s="178"/>
+      <c r="D26" s="181"/>
+      <c r="E26" s="181"/>
+      <c r="F26" s="181"/>
+      <c r="G26" s="181"/>
+      <c r="H26" s="181"/>
+      <c r="I26" s="181"/>
+      <c r="J26" s="181"/>
+      <c r="K26" s="182"/>
     </row>
     <row r="27" spans="1:11" ht="256.5" customHeight="1">
       <c r="A27" s="76">
@@ -5634,17 +5681,17 @@
       <c r="B27" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="176" t="s">
+      <c r="C27" s="180" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="177"/>
-      <c r="E27" s="177"/>
-      <c r="F27" s="177"/>
-      <c r="G27" s="177"/>
-      <c r="H27" s="177"/>
-      <c r="I27" s="177"/>
-      <c r="J27" s="177"/>
-      <c r="K27" s="178"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="181"/>
+      <c r="I27" s="181"/>
+      <c r="J27" s="181"/>
+      <c r="K27" s="182"/>
     </row>
     <row r="28" spans="1:11" ht="185.25" customHeight="1">
       <c r="A28" s="76">
@@ -5653,17 +5700,17 @@
       <c r="B28" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="176" t="s">
+      <c r="C28" s="180" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="177"/>
-      <c r="E28" s="177"/>
-      <c r="F28" s="177"/>
-      <c r="G28" s="177"/>
-      <c r="H28" s="177"/>
-      <c r="I28" s="177"/>
-      <c r="J28" s="177"/>
-      <c r="K28" s="178"/>
+      <c r="D28" s="181"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="181"/>
+      <c r="G28" s="181"/>
+      <c r="H28" s="181"/>
+      <c r="I28" s="181"/>
+      <c r="J28" s="181"/>
+      <c r="K28" s="182"/>
     </row>
     <row r="29" spans="1:11" ht="156.75" customHeight="1">
       <c r="A29" s="76">
@@ -5672,17 +5719,17 @@
       <c r="B29" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="176" t="s">
+      <c r="C29" s="180" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="177"/>
-      <c r="E29" s="177"/>
-      <c r="F29" s="177"/>
-      <c r="G29" s="177"/>
-      <c r="H29" s="177"/>
-      <c r="I29" s="177"/>
-      <c r="J29" s="177"/>
-      <c r="K29" s="178"/>
+      <c r="D29" s="181"/>
+      <c r="E29" s="181"/>
+      <c r="F29" s="181"/>
+      <c r="G29" s="181"/>
+      <c r="H29" s="181"/>
+      <c r="I29" s="181"/>
+      <c r="J29" s="181"/>
+      <c r="K29" s="182"/>
     </row>
     <row r="30" spans="1:11" ht="213.75" customHeight="1">
       <c r="A30" s="76">
@@ -5691,17 +5738,17 @@
       <c r="B30" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="176" t="s">
+      <c r="C30" s="180" t="s">
         <v>134</v>
       </c>
-      <c r="D30" s="177"/>
-      <c r="E30" s="177"/>
-      <c r="F30" s="177"/>
-      <c r="G30" s="177"/>
-      <c r="H30" s="177"/>
-      <c r="I30" s="177"/>
-      <c r="J30" s="177"/>
-      <c r="K30" s="178"/>
+      <c r="D30" s="181"/>
+      <c r="E30" s="181"/>
+      <c r="F30" s="181"/>
+      <c r="G30" s="181"/>
+      <c r="H30" s="181"/>
+      <c r="I30" s="181"/>
+      <c r="J30" s="181"/>
+      <c r="K30" s="182"/>
     </row>
     <row r="31" spans="1:11" ht="114" customHeight="1">
       <c r="A31" s="76">
@@ -5710,17 +5757,17 @@
       <c r="B31" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="176" t="s">
+      <c r="C31" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="177"/>
-      <c r="E31" s="177"/>
-      <c r="F31" s="177"/>
-      <c r="G31" s="177"/>
-      <c r="H31" s="177"/>
-      <c r="I31" s="177"/>
-      <c r="J31" s="177"/>
-      <c r="K31" s="178"/>
+      <c r="D31" s="181"/>
+      <c r="E31" s="181"/>
+      <c r="F31" s="181"/>
+      <c r="G31" s="181"/>
+      <c r="H31" s="181"/>
+      <c r="I31" s="181"/>
+      <c r="J31" s="181"/>
+      <c r="K31" s="182"/>
     </row>
     <row r="32" spans="1:11" ht="99.75" customHeight="1">
       <c r="A32" s="76">
@@ -5729,17 +5776,17 @@
       <c r="B32" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="176" t="s">
+      <c r="C32" s="180" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="177"/>
-      <c r="E32" s="177"/>
-      <c r="F32" s="177"/>
-      <c r="G32" s="177"/>
-      <c r="H32" s="177"/>
-      <c r="I32" s="177"/>
-      <c r="J32" s="177"/>
-      <c r="K32" s="178"/>
+      <c r="D32" s="181"/>
+      <c r="E32" s="181"/>
+      <c r="F32" s="181"/>
+      <c r="G32" s="181"/>
+      <c r="H32" s="181"/>
+      <c r="I32" s="181"/>
+      <c r="J32" s="181"/>
+      <c r="K32" s="182"/>
     </row>
     <row r="33" spans="1:11" ht="171" customHeight="1">
       <c r="A33" s="76">
@@ -5748,17 +5795,17 @@
       <c r="B33" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="176" t="s">
+      <c r="C33" s="180" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="177"/>
-      <c r="E33" s="177"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="177"/>
-      <c r="H33" s="177"/>
-      <c r="I33" s="177"/>
-      <c r="J33" s="177"/>
-      <c r="K33" s="178"/>
+      <c r="D33" s="181"/>
+      <c r="E33" s="181"/>
+      <c r="F33" s="181"/>
+      <c r="G33" s="181"/>
+      <c r="H33" s="181"/>
+      <c r="I33" s="181"/>
+      <c r="J33" s="181"/>
+      <c r="K33" s="182"/>
     </row>
     <row r="34" spans="1:11" ht="171" customHeight="1">
       <c r="A34" s="76">
@@ -5767,17 +5814,17 @@
       <c r="B34" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="C34" s="176" t="s">
+      <c r="C34" s="180" t="s">
         <v>142</v>
       </c>
-      <c r="D34" s="177"/>
-      <c r="E34" s="177"/>
-      <c r="F34" s="177"/>
-      <c r="G34" s="177"/>
-      <c r="H34" s="177"/>
-      <c r="I34" s="177"/>
-      <c r="J34" s="177"/>
-      <c r="K34" s="178"/>
+      <c r="D34" s="181"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="181"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="181"/>
+      <c r="I34" s="181"/>
+      <c r="J34" s="181"/>
+      <c r="K34" s="182"/>
     </row>
     <row r="35" spans="1:11" ht="111.75" customHeight="1" thickBot="1">
       <c r="A35" s="77">
@@ -5786,17 +5833,17 @@
       <c r="B35" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="179" t="s">
+      <c r="C35" s="183" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="180"/>
-      <c r="E35" s="180"/>
-      <c r="F35" s="180"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="180"/>
-      <c r="J35" s="180"/>
-      <c r="K35" s="181"/>
+      <c r="D35" s="184"/>
+      <c r="E35" s="184"/>
+      <c r="F35" s="184"/>
+      <c r="G35" s="184"/>
+      <c r="H35" s="184"/>
+      <c r="I35" s="184"/>
+      <c r="J35" s="184"/>
+      <c r="K35" s="185"/>
     </row>
     <row r="36" spans="1:11" ht="15" thickTop="1"/>
   </sheetData>
@@ -5826,7 +5873,7 @@
   <dimension ref="A2:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="C44" sqref="C44:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5837,12 +5884,12 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A2" s="27"/>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="188" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -6279,7 +6326,7 @@
   <dimension ref="A2:O18"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6295,22 +6342,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="48.75" customHeight="1" thickBot="1">
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="190" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="187"/>
-      <c r="I2" s="187"/>
-      <c r="J2" s="187"/>
-      <c r="K2" s="187"/>
-      <c r="L2" s="187"/>
-      <c r="M2" s="187"/>
-      <c r="N2" s="187"/>
-      <c r="O2" s="187"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="191"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickTop="1"/>
     <row r="4" spans="1:15" ht="36" customHeight="1">
@@ -6344,19 +6391,19 @@
       <c r="D5" s="64"/>
       <c r="E5" s="64">
         <f>SUM(E7:E15)</f>
-        <v>15</v>
+        <v>13.5</v>
       </c>
       <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:15" ht="18.75">
-      <c r="A6" s="57"/>
-      <c r="B6" s="89" t="s">
+      <c r="A6" s="67"/>
+      <c r="B6" s="193" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="48"/>
+      <c r="C6" s="194"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="85"/>
       <c r="H6" s="23" t="s">
         <v>217</v>
       </c>
@@ -6381,11 +6428,11 @@
         <v>1.5</v>
       </c>
       <c r="D7" s="64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="64">
         <f xml:space="preserve"> C7 * D7</f>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F7" s="48">
         <f>IF(E7&lt;=0,0,IF(E7&lt;=1,0.05,IF(E7&lt;=2,0.1,IF(E7&lt;=3,0.6,1))))</f>
@@ -6422,7 +6469,7 @@
         <v>1.5</v>
       </c>
       <c r="F8" s="48">
-        <f t="shared" ref="F7:F15" si="1">IF(E8&lt;=0,0,IF(E8&lt;=1,0.05,IF(E8&lt;=2,0.1,IF(E8&lt;=3,0.6,1))))</f>
+        <f t="shared" ref="F8:F15" si="1">IF(E8&lt;=0,0,IF(E8&lt;=1,0.05,IF(E8&lt;=2,0.1,IF(E8&lt;=3,0.6,1))))</f>
         <v>0.1</v>
       </c>
       <c r="H8" s="39" t="s">
@@ -6518,7 +6565,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="48">
-        <f t="shared" si="1"/>
+        <f>IF(E11&lt;=0,0,IF(E11&lt;=1,0.05,IF(E11&lt;=2,0.1,IF(E11&lt;=3,0.6,1))))</f>
         <v>1</v>
       </c>
       <c r="H11" s="87" t="s">
@@ -6529,20 +6576,14 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" thickTop="1">
-      <c r="A12" s="57"/>
-      <c r="B12" s="89" t="s">
+      <c r="A12" s="67"/>
+      <c r="B12" s="193" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C12" s="194"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="85"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="57">
@@ -6655,21 +6696,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f12cf464957118729b6c32269c3bef6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3cd9a7ce2c5f9b2e78bd9172391e822" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -6860,32 +6886,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83ECEE42-EE99-4ABB-9150-2CE624452AEC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{694905DF-9CBA-43C2-8859-CF2BE00A6E2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774330F1-64B3-4F0E-BB4B-6A27A48AFFF9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6902,4 +6918,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{694905DF-9CBA-43C2-8859-CF2BE00A6E2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83ECEE42-EE99-4ABB-9150-2CE624452AEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Chặn copy hoặc xem mã nguồn trên website. - Bật bảo trì hệ thống đến khi triển khai. - Chuyển vào giai đoạn alpha test.
</commit_message>
<xml_diff>
--- a/Docs/Report/Tính giá trị phần mềm web hỗ trợ tuyển sinh.xlsx
+++ b/Docs/Report/Tính giá trị phần mềm web hỗ trợ tuyển sinh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Giá trị phần mềm" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="244">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -816,6 +816,9 @@
   <si>
     <t>Hiển thị cờ theo năm</t>
   </si>
+  <si>
+    <t>Xem nhật kí tương tác</t>
+  </si>
 </sst>
 </file>
 
@@ -827,7 +830,7 @@
     <numFmt numFmtId="166" formatCode="#,##0\ [$VND/người/giờ]"/>
     <numFmt numFmtId="167" formatCode="0.00\ [$giờ]"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="#,##0\ [$VND]"/>
+    <numFmt numFmtId="169" formatCode="#,##0\ [$VND]"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -2009,6 +2012,15 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2108,6 +2120,15 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2124,6 +2145,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2233,27 +2257,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3266,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -3295,10 +3298,10 @@
       <c r="D2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="142" t="s">
+      <c r="E2" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="142"/>
+      <c r="F2" s="145"/>
     </row>
     <row r="3" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="B3" s="1" t="s">
@@ -3307,10 +3310,10 @@
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="143">
+      <c r="E3" s="146">
         <v>43413</v>
       </c>
-      <c r="F3" s="143"/>
+      <c r="F3" s="146"/>
     </row>
     <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="12" t="s">
@@ -3322,11 +3325,11 @@
       <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="9" spans="1:8" ht="30" customHeight="1">
@@ -3339,11 +3342,11 @@
       <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
     </row>
     <row r="10" spans="1:8" ht="45.75" customHeight="1">
       <c r="A10" s="14" t="s">
@@ -3355,12 +3358,12 @@
       <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="117">
+      <c r="D10" s="120">
         <f>E</f>
-        <v>167.50824999999998</v>
-      </c>
-      <c r="E10" s="118"/>
-      <c r="F10" s="119"/>
+        <v>171.19666666666663</v>
+      </c>
+      <c r="E10" s="121"/>
+      <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:8" ht="45.75" customHeight="1">
       <c r="A11" s="15" t="s">
@@ -3372,12 +3375,12 @@
       <c r="C11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="144">
+      <c r="D11" s="147">
         <f>'Phụlục VI-2'!F17</f>
-        <v>20</v>
-      </c>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
+        <v>32</v>
+      </c>
+      <c r="E11" s="148"/>
+      <c r="F11" s="149"/>
     </row>
     <row r="12" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
       <c r="A12" s="15" t="s">
@@ -3389,30 +3392,30 @@
       <c r="C12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="147">
+      <c r="D12" s="150">
         <v>20000</v>
       </c>
-      <c r="E12" s="148"/>
-      <c r="F12" s="149"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="152"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1">
       <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="195">
+      <c r="D14" s="153">
         <f xml:space="preserve"> 1.4 * D10 * D11 * D12 * 1.1</f>
-        <v>103185081.99999997</v>
-      </c>
-      <c r="E14" s="196"/>
-      <c r="F14" s="197"/>
+        <v>168731434.66666663</v>
+      </c>
+      <c r="E14" s="154"/>
+      <c r="F14" s="155"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
       <c r="A15" s="9" t="s">
@@ -3421,14 +3424,14 @@
       <c r="C15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="150">
-        <v>0</v>
-      </c>
-      <c r="E15" s="151" t="e">
+      <c r="D15" s="156">
+        <v>-4000000</v>
+      </c>
+      <c r="E15" s="157" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="F15" s="152"/>
+      <c r="F15" s="158"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="24" customHeight="1">
@@ -3438,25 +3441,25 @@
       <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="153">
+      <c r="D16" s="159">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="160">
         <v>0</v>
       </c>
-      <c r="E16" s="154">
-        <v>0</v>
-      </c>
-      <c r="F16" s="155"/>
+      <c r="F16" s="161"/>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="24" customHeight="1">
       <c r="C17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="198">
+      <c r="D17" s="162">
         <f>(D14+D15)*(1-D16)</f>
-        <v>103185081.99999997</v>
-      </c>
-      <c r="E17" s="198"/>
-      <c r="F17" s="198"/>
+        <v>148258291.19999996</v>
+      </c>
+      <c r="E17" s="162"/>
+      <c r="F17" s="162"/>
     </row>
     <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8"/>
@@ -3470,11 +3473,11 @@
       <c r="F19" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B21" s="140" t="s">
+      <c r="B21" s="143" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
+      <c r="C21" s="144"/>
+      <c r="D21" s="144"/>
     </row>
     <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="23" spans="1:6" ht="30" customHeight="1">
@@ -3487,11 +3490,11 @@
       <c r="C23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="129" t="s">
+      <c r="D23" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
     </row>
     <row r="24" spans="1:6" ht="45.75" customHeight="1" thickBot="1">
       <c r="A24" s="15" t="s">
@@ -3503,31 +3506,31 @@
       <c r="C24" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="117">
+      <c r="D24" s="120">
         <f>AUCP</f>
-        <v>100.50494999999998</v>
-      </c>
-      <c r="E24" s="118"/>
-      <c r="F24" s="119"/>
+        <v>102.71799999999998</v>
+      </c>
+      <c r="E24" s="121"/>
+      <c r="F24" s="122"/>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="123"/>
     </row>
     <row r="26" spans="1:6" ht="24" customHeight="1" thickBot="1">
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="121">
+      <c r="D26" s="124">
         <f>10 / 6 * D24</f>
-        <v>167.50824999999998</v>
-      </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="123"/>
+        <v>171.19666666666663</v>
+      </c>
+      <c r="E26" s="125"/>
+      <c r="F26" s="126"/>
     </row>
     <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3558,11 +3561,11 @@
       <c r="C32" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="129" t="s">
+      <c r="D32" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="130"/>
-      <c r="F32" s="130"/>
+      <c r="E32" s="133"/>
+      <c r="F32" s="133"/>
     </row>
     <row r="33" spans="1:7" ht="45.75" customHeight="1">
       <c r="A33" s="15" t="s">
@@ -3572,12 +3575,12 @@
         <v>33</v>
       </c>
       <c r="C33" s="16"/>
-      <c r="D33" s="117">
+      <c r="D33" s="120">
         <f>UUCP</f>
-        <v>111</v>
-      </c>
-      <c r="E33" s="118"/>
-      <c r="F33" s="119"/>
+        <v>116</v>
+      </c>
+      <c r="E33" s="121"/>
+      <c r="F33" s="122"/>
     </row>
     <row r="34" spans="1:7" ht="45.75" customHeight="1">
       <c r="A34" s="15" t="s">
@@ -3587,12 +3590,12 @@
         <v>34</v>
       </c>
       <c r="C34" s="16"/>
-      <c r="D34" s="137">
+      <c r="D34" s="140">
         <f>TCF</f>
-        <v>0.90999999999999992</v>
-      </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="139"/>
+        <v>0.7</v>
+      </c>
+      <c r="E34" s="141"/>
+      <c r="F34" s="142"/>
     </row>
     <row r="35" spans="1:7" ht="45.75" customHeight="1" thickBot="1">
       <c r="A35" s="15" t="s">
@@ -3602,31 +3605,31 @@
         <v>35</v>
       </c>
       <c r="C35" s="16"/>
-      <c r="D35" s="134">
+      <c r="D35" s="137">
         <f>EF</f>
-        <v>0.99499999999999988</v>
-      </c>
-      <c r="E35" s="135"/>
-      <c r="F35" s="136"/>
+        <v>1.2649999999999999</v>
+      </c>
+      <c r="E35" s="138"/>
+      <c r="F35" s="139"/>
     </row>
     <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="120"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
     </row>
     <row r="37" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="C37" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="121">
+      <c r="D37" s="124">
         <f xml:space="preserve"> D33 * D34 * D35</f>
-        <v>100.50494999999998</v>
-      </c>
-      <c r="E37" s="122"/>
-      <c r="F37" s="123"/>
+        <v>102.71799999999998</v>
+      </c>
+      <c r="E37" s="125"/>
+      <c r="F37" s="126"/>
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3657,11 +3660,11 @@
       <c r="C43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="129" t="s">
+      <c r="D43" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130"/>
+      <c r="E43" s="133"/>
+      <c r="F43" s="133"/>
     </row>
     <row r="44" spans="1:7" ht="45.75" customHeight="1">
       <c r="A44" s="15" t="s">
@@ -3673,12 +3676,12 @@
       <c r="C44" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="117">
+      <c r="D44" s="120">
         <f>'Phụ lục III'!E8</f>
         <v>6</v>
       </c>
-      <c r="E44" s="118"/>
-      <c r="F44" s="119"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="122"/>
       <c r="G44" s="1" t="s">
         <v>69</v>
       </c>
@@ -3693,12 +3696,12 @@
       <c r="C45" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="131">
+      <c r="D45" s="134">
         <f>'Phụ lục IV'!D17:F17</f>
-        <v>105</v>
-      </c>
-      <c r="E45" s="132"/>
-      <c r="F45" s="133"/>
+        <v>110</v>
+      </c>
+      <c r="E45" s="135"/>
+      <c r="F45" s="136"/>
       <c r="G45" s="1" t="s">
         <v>70</v>
       </c>
@@ -3707,20 +3710,20 @@
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="120"/>
-      <c r="E46" s="120"/>
-      <c r="F46" s="120"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="123"/>
     </row>
     <row r="47" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="C47" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="121">
+      <c r="D47" s="124">
         <f xml:space="preserve"> D44 + D45</f>
-        <v>111</v>
-      </c>
-      <c r="E47" s="122"/>
-      <c r="F47" s="123"/>
+        <v>116</v>
+      </c>
+      <c r="E47" s="125"/>
+      <c r="F47" s="126"/>
     </row>
     <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3732,13 +3735,13 @@
       <c r="F49" s="17"/>
     </row>
     <row r="51" spans="1:7" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B51" s="127" t="s">
+      <c r="B51" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="128"/>
-      <c r="D51" s="128"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="128"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="131"/>
     </row>
     <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="53" spans="1:7" ht="30" customHeight="1">
@@ -3751,11 +3754,11 @@
       <c r="C53" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="129" t="s">
+      <c r="D53" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="130"/>
-      <c r="F53" s="130"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="133"/>
     </row>
     <row r="54" spans="1:7" ht="45.75" customHeight="1" thickBot="1">
       <c r="A54" s="15" t="s">
@@ -3767,12 +3770,12 @@
       <c r="C54" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="117">
+      <c r="D54" s="120">
         <f>'Phụ lục V'!E5</f>
-        <v>31</v>
-      </c>
-      <c r="E54" s="118"/>
-      <c r="F54" s="119"/>
+        <v>10</v>
+      </c>
+      <c r="E54" s="121"/>
+      <c r="F54" s="122"/>
       <c r="G54" s="1" t="s">
         <v>117</v>
       </c>
@@ -3781,20 +3784,20 @@
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="120"/>
-      <c r="E55" s="120"/>
-      <c r="F55" s="120"/>
+      <c r="D55" s="123"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="123"/>
     </row>
     <row r="56" spans="1:7" ht="24" customHeight="1" thickBot="1">
       <c r="C56" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D56" s="124">
+      <c r="D56" s="127">
         <f>0.6 + (0.01 * D54)</f>
-        <v>0.90999999999999992</v>
-      </c>
-      <c r="E56" s="125"/>
-      <c r="F56" s="126"/>
+        <v>0.7</v>
+      </c>
+      <c r="E56" s="128"/>
+      <c r="F56" s="129"/>
     </row>
     <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3806,13 +3809,13 @@
       <c r="F58" s="17"/>
     </row>
     <row r="60" spans="1:7" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B60" s="127" t="s">
+      <c r="B60" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="128"/>
-      <c r="D60" s="128"/>
-      <c r="E60" s="128"/>
-      <c r="F60" s="128"/>
+      <c r="C60" s="131"/>
+      <c r="D60" s="131"/>
+      <c r="E60" s="131"/>
+      <c r="F60" s="131"/>
     </row>
     <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="62" spans="1:7" ht="30" customHeight="1">
@@ -3825,11 +3828,11 @@
       <c r="C62" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="129" t="s">
+      <c r="D62" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="130"/>
-      <c r="F62" s="130"/>
+      <c r="E62" s="133"/>
+      <c r="F62" s="133"/>
     </row>
     <row r="63" spans="1:7" ht="45.75" customHeight="1" thickBot="1">
       <c r="A63" s="15" t="s">
@@ -3841,12 +3844,12 @@
       <c r="C63" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D63" s="117">
+      <c r="D63" s="120">
         <f>'Phụlục VI-2'!E5</f>
-        <v>13.5</v>
-      </c>
-      <c r="E63" s="118"/>
-      <c r="F63" s="119"/>
+        <v>4.5</v>
+      </c>
+      <c r="E63" s="121"/>
+      <c r="F63" s="122"/>
       <c r="G63" s="1" t="s">
         <v>218</v>
       </c>
@@ -3855,20 +3858,20 @@
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="120"/>
-      <c r="E64" s="120"/>
-      <c r="F64" s="120"/>
+      <c r="D64" s="123"/>
+      <c r="E64" s="123"/>
+      <c r="F64" s="123"/>
     </row>
     <row r="65" spans="3:6" ht="24" customHeight="1" thickBot="1">
       <c r="C65" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D65" s="121">
+      <c r="D65" s="124">
         <f>1.4 + (-0.03 * D63)</f>
-        <v>0.99499999999999988</v>
-      </c>
-      <c r="E65" s="122"/>
-      <c r="F65" s="123"/>
+        <v>1.2649999999999999</v>
+      </c>
+      <c r="E65" s="125"/>
+      <c r="F65" s="126"/>
     </row>
     <row r="66" spans="3:6" ht="20.100000000000001" customHeight="1" thickTop="1"/>
   </sheetData>
@@ -3960,7 +3963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D22" sqref="D22:F22"/>
     </sheetView>
   </sheetViews>
@@ -3999,11 +4002,11 @@
       <c r="C4" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="156" t="s">
+      <c r="D4" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
     </row>
     <row r="5" spans="1:12" ht="39.75" customHeight="1">
       <c r="A5" s="39">
@@ -4011,9 +4014,9 @@
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="29"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="159"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="166"/>
     </row>
     <row r="6" spans="1:12" ht="39.75" customHeight="1">
       <c r="A6" s="39">
@@ -4161,9 +4164,9 @@
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="29"/>
-      <c r="D20" s="160"/>
-      <c r="E20" s="161"/>
-      <c r="F20" s="162"/>
+      <c r="D20" s="167"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="169"/>
     </row>
     <row r="21" spans="1:6" ht="39.75" customHeight="1">
       <c r="A21" s="39">
@@ -4171,9 +4174,9 @@
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="29"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="164"/>
-      <c r="F21" s="165"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="171"/>
+      <c r="F21" s="172"/>
     </row>
     <row r="22" spans="1:6" ht="39.75" customHeight="1" thickBot="1">
       <c r="A22" s="40">
@@ -4181,9 +4184,9 @@
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="32"/>
-      <c r="D22" s="166"/>
-      <c r="E22" s="167"/>
-      <c r="F22" s="168"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="175"/>
     </row>
     <row r="23" spans="1:6" ht="15" thickTop="1"/>
     <row r="24" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -4210,10 +4213,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G27"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G25" sqref="G5:G25"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4226,13 +4229,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="176" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickTop="1">
       <c r="A3" s="38"/>
@@ -4463,7 +4466,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>240</v>
@@ -4480,7 +4483,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C17" s="62" t="s">
         <v>240</v>
@@ -4497,7 +4500,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C18" s="62" t="s">
         <v>240</v>
@@ -4514,10 +4517,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D19" s="102"/>
       <c r="E19" s="102"/>
@@ -4531,7 +4534,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C20" s="62" t="s">
         <v>239</v>
@@ -4548,24 +4551,24 @@
         <v>17</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="D21" s="104"/>
-      <c r="E21" s="105"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
       <c r="F21" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="G21" s="192"/>
+      <c r="G21" s="103"/>
     </row>
     <row r="22" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
       <c r="A22" s="57">
         <v>18</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C22" s="62" t="s">
         <v>239</v>
@@ -4575,14 +4578,14 @@
       <c r="F22" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="192"/>
+      <c r="G22" s="117"/>
     </row>
     <row r="23" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
       <c r="A23" s="57">
         <v>19</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>239</v>
@@ -4592,50 +4595,67 @@
       <c r="F23" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="192"/>
+      <c r="G23" s="117"/>
     </row>
     <row r="24" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
       <c r="A24" s="57">
         <v>20</v>
       </c>
-      <c r="B24" s="112" t="s">
-        <v>237</v>
+      <c r="B24" s="58" t="s">
+        <v>236</v>
       </c>
       <c r="C24" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="105"/>
       <c r="F24" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="192"/>
-    </row>
-    <row r="25" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A25" s="60">
+      <c r="G24" s="117"/>
+    </row>
+    <row r="25" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A25" s="57">
         <v>21</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="112" t="s">
+        <v>237</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="109" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="117"/>
+    </row>
+    <row r="26" spans="1:7" s="101" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
+      <c r="A26" s="57">
+        <v>22</v>
+      </c>
+      <c r="B26" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="C25" s="106" t="s">
+      <c r="C26" s="106" t="s">
         <v>239</v>
       </c>
-      <c r="D25" s="106"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="115" t="s">
+      <c r="D26" s="106"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="192"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickTop="1"/>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="108"/>
-      <c r="C27" s="108"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
-      <c r="F27" s="110"/>
+      <c r="G26" s="117"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickTop="1"/>
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A28" s="17"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4667,13 +4687,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="48.75" customHeight="1" thickBot="1">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1">
       <c r="A3" s="38"/>
@@ -4834,8 +4854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4851,18 +4871,18 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="47.25" customHeight="1" thickBot="1">
       <c r="A2" s="22"/>
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="176" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickTop="1"/>
@@ -4876,11 +4896,11 @@
       <c r="C4" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="176" t="s">
+      <c r="D4" s="183" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
       <c r="H4" s="23" t="s">
         <v>58</v>
       </c>
@@ -4902,12 +4922,12 @@
         <v>89</v>
       </c>
       <c r="C5" s="69"/>
-      <c r="D5" s="177">
+      <c r="D5" s="184">
         <f>SUM(D6:F8)</f>
-        <v>105</v>
-      </c>
-      <c r="E5" s="178"/>
-      <c r="F5" s="179"/>
+        <v>110</v>
+      </c>
+      <c r="E5" s="185"/>
+      <c r="F5" s="186"/>
       <c r="H5" s="57">
         <v>1</v>
       </c>
@@ -4923,14 +4943,14 @@
         <v>90</v>
       </c>
       <c r="C6" s="47">
-        <v>21</v>
-      </c>
-      <c r="D6" s="157">
+        <v>22</v>
+      </c>
+      <c r="D6" s="164">
         <f>C6 * J6 * K6</f>
-        <v>105</v>
-      </c>
-      <c r="E6" s="158"/>
-      <c r="F6" s="159"/>
+        <v>110</v>
+      </c>
+      <c r="E6" s="165"/>
+      <c r="F6" s="166"/>
       <c r="H6" s="57"/>
       <c r="I6" s="62" t="s">
         <v>90</v>
@@ -4950,12 +4970,12 @@
       <c r="C7" s="47">
         <v>0</v>
       </c>
-      <c r="D7" s="157">
+      <c r="D7" s="164">
         <f>C7 * J7 * K7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="158"/>
-      <c r="F7" s="159"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="166"/>
       <c r="H7" s="57"/>
       <c r="I7" s="62" t="s">
         <v>91</v>
@@ -4975,12 +4995,12 @@
       <c r="C8" s="47">
         <v>0</v>
       </c>
-      <c r="D8" s="157">
+      <c r="D8" s="164">
         <f>C8 * J8 * K8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="158"/>
-      <c r="F8" s="159"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="166"/>
       <c r="H8" s="57"/>
       <c r="I8" s="62" t="s">
         <v>92</v>
@@ -5000,12 +5020,12 @@
         <v>93</v>
       </c>
       <c r="C9" s="69"/>
-      <c r="D9" s="172">
+      <c r="D9" s="179">
         <f>SUM(D10:F12)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="173"/>
-      <c r="F9" s="174"/>
+      <c r="E9" s="180"/>
+      <c r="F9" s="181"/>
       <c r="H9" s="57">
         <v>2</v>
       </c>
@@ -5023,12 +5043,12 @@
       <c r="C10" s="47">
         <v>0</v>
       </c>
-      <c r="D10" s="157">
+      <c r="D10" s="164">
         <f>C10 * J10 * K10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="158"/>
-      <c r="F10" s="159"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="166"/>
       <c r="H10" s="57"/>
       <c r="I10" s="62" t="s">
         <v>90</v>
@@ -5048,12 +5068,12 @@
       <c r="C11" s="47">
         <v>0</v>
       </c>
-      <c r="D11" s="157">
+      <c r="D11" s="164">
         <f>C11 * J11 * K11</f>
         <v>0</v>
       </c>
-      <c r="E11" s="158"/>
-      <c r="F11" s="159"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="166"/>
       <c r="H11" s="57"/>
       <c r="I11" s="62" t="s">
         <v>91</v>
@@ -5073,12 +5093,12 @@
       <c r="C12" s="47">
         <v>0</v>
       </c>
-      <c r="D12" s="157">
+      <c r="D12" s="164">
         <f>C12 * J12 * K12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="158"/>
-      <c r="F12" s="159"/>
+      <c r="E12" s="165"/>
+      <c r="F12" s="166"/>
       <c r="H12" s="57"/>
       <c r="I12" s="62" t="s">
         <v>92</v>
@@ -5098,12 +5118,12 @@
         <v>94</v>
       </c>
       <c r="C13" s="69"/>
-      <c r="D13" s="172">
+      <c r="D13" s="179">
         <f>SUM(D14:F16)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="174"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="181"/>
       <c r="H13" s="57">
         <v>3</v>
       </c>
@@ -5121,12 +5141,12 @@
       <c r="C14" s="47">
         <v>0</v>
       </c>
-      <c r="D14" s="157">
+      <c r="D14" s="164">
         <f>C14 * J14 * K14</f>
         <v>0</v>
       </c>
-      <c r="E14" s="158"/>
-      <c r="F14" s="159"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="166"/>
       <c r="H14" s="57"/>
       <c r="I14" s="62" t="s">
         <v>90</v>
@@ -5146,12 +5166,12 @@
       <c r="C15" s="47">
         <v>0</v>
       </c>
-      <c r="D15" s="157">
+      <c r="D15" s="164">
         <f>C15 * J15 * K15</f>
         <v>0</v>
       </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="159"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="166"/>
       <c r="H15" s="57"/>
       <c r="I15" s="62" t="s">
         <v>91</v>
@@ -5171,12 +5191,12 @@
       <c r="C16" s="47">
         <v>0</v>
       </c>
-      <c r="D16" s="157">
+      <c r="D16" s="164">
         <f>C16 * J16 * K16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="158"/>
-      <c r="F16" s="159"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="166"/>
       <c r="H16" s="59"/>
       <c r="I16" s="63" t="s">
         <v>92</v>
@@ -5198,12 +5218,12 @@
       <c r="C17" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="170">
+      <c r="D17" s="177">
         <f xml:space="preserve"> D5 + D9 + D13</f>
-        <v>105</v>
-      </c>
-      <c r="E17" s="135"/>
-      <c r="F17" s="171"/>
+        <v>110</v>
+      </c>
+      <c r="E17" s="138"/>
+      <c r="F17" s="178"/>
     </row>
     <row r="18" spans="1:11" ht="15" thickTop="1"/>
     <row r="19" spans="1:11" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -5246,8 +5266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5263,13 +5283,13 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A2" s="22"/>
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="176" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -5313,7 +5333,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="116">
         <f xml:space="preserve"> SUM(E6:E18)</f>
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F5" s="74"/>
     </row>
@@ -5328,11 +5348,11 @@
         <v>2</v>
       </c>
       <c r="D6" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" s="116">
         <f t="shared" ref="E6:E18" si="0">D6 * C6</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6" s="74"/>
     </row>
@@ -5347,11 +5367,11 @@
         <v>1</v>
       </c>
       <c r="D7" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="116">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="74"/>
     </row>
@@ -5366,11 +5386,11 @@
         <v>1</v>
       </c>
       <c r="D8" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="116">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="74"/>
     </row>
@@ -5385,11 +5405,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="116">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F9" s="74"/>
     </row>
@@ -5404,11 +5424,11 @@
         <v>1</v>
       </c>
       <c r="D10" s="43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="116">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" s="74"/>
     </row>
@@ -5423,11 +5443,11 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="116">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F11" s="74"/>
     </row>
@@ -5442,11 +5462,11 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="116">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F12" s="74"/>
     </row>
@@ -5461,11 +5481,11 @@
         <v>2</v>
       </c>
       <c r="D13" s="43">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13" s="116">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F13" s="74"/>
     </row>
@@ -5480,11 +5500,11 @@
         <v>1</v>
       </c>
       <c r="D14" s="43">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" s="116">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14" s="74"/>
     </row>
@@ -5499,11 +5519,11 @@
         <v>1</v>
       </c>
       <c r="D15" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="116">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="74"/>
     </row>
@@ -5518,11 +5538,11 @@
         <v>1</v>
       </c>
       <c r="D16" s="43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="116">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="74"/>
     </row>
@@ -5537,11 +5557,11 @@
         <v>1</v>
       </c>
       <c r="D17" s="43">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="116">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F17" s="74"/>
     </row>
@@ -5586,17 +5606,17 @@
       <c r="B22" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="186" t="s">
+      <c r="C22" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="187"/>
-      <c r="E22" s="187"/>
-      <c r="F22" s="187"/>
-      <c r="G22" s="187"/>
-      <c r="H22" s="187"/>
-      <c r="I22" s="187"/>
-      <c r="J22" s="187"/>
-      <c r="K22" s="187"/>
+      <c r="D22" s="194"/>
+      <c r="E22" s="194"/>
+      <c r="F22" s="194"/>
+      <c r="G22" s="194"/>
+      <c r="H22" s="194"/>
+      <c r="I22" s="194"/>
+      <c r="J22" s="194"/>
+      <c r="K22" s="194"/>
     </row>
     <row r="23" spans="1:11" ht="99.75" customHeight="1">
       <c r="A23" s="76">
@@ -5605,17 +5625,17 @@
       <c r="B23" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="180" t="s">
+      <c r="C23" s="187" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="181"/>
-      <c r="E23" s="181"/>
-      <c r="F23" s="181"/>
-      <c r="G23" s="181"/>
-      <c r="H23" s="181"/>
-      <c r="I23" s="181"/>
-      <c r="J23" s="181"/>
-      <c r="K23" s="182"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="188"/>
+      <c r="K23" s="189"/>
     </row>
     <row r="24" spans="1:11" ht="142.5" customHeight="1">
       <c r="A24" s="76">
@@ -5624,17 +5644,17 @@
       <c r="B24" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="180" t="s">
+      <c r="C24" s="187" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="182"/>
+      <c r="D24" s="188"/>
+      <c r="E24" s="188"/>
+      <c r="F24" s="188"/>
+      <c r="G24" s="188"/>
+      <c r="H24" s="188"/>
+      <c r="I24" s="188"/>
+      <c r="J24" s="188"/>
+      <c r="K24" s="189"/>
     </row>
     <row r="25" spans="1:11" ht="99.75" customHeight="1">
       <c r="A25" s="76">
@@ -5643,17 +5663,17 @@
       <c r="B25" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="180" t="s">
+      <c r="C25" s="187" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="181"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="181"/>
-      <c r="H25" s="181"/>
-      <c r="I25" s="181"/>
-      <c r="J25" s="181"/>
-      <c r="K25" s="182"/>
+      <c r="D25" s="188"/>
+      <c r="E25" s="188"/>
+      <c r="F25" s="188"/>
+      <c r="G25" s="188"/>
+      <c r="H25" s="188"/>
+      <c r="I25" s="188"/>
+      <c r="J25" s="188"/>
+      <c r="K25" s="189"/>
     </row>
     <row r="26" spans="1:11" ht="142.5" customHeight="1">
       <c r="A26" s="76">
@@ -5662,17 +5682,17 @@
       <c r="B26" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="180" t="s">
+      <c r="C26" s="187" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="181"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181"/>
-      <c r="I26" s="181"/>
-      <c r="J26" s="181"/>
-      <c r="K26" s="182"/>
+      <c r="D26" s="188"/>
+      <c r="E26" s="188"/>
+      <c r="F26" s="188"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="188"/>
+      <c r="I26" s="188"/>
+      <c r="J26" s="188"/>
+      <c r="K26" s="189"/>
     </row>
     <row r="27" spans="1:11" ht="256.5" customHeight="1">
       <c r="A27" s="76">
@@ -5681,17 +5701,17 @@
       <c r="B27" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="180" t="s">
+      <c r="C27" s="187" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="181"/>
-      <c r="K27" s="182"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
+      <c r="G27" s="188"/>
+      <c r="H27" s="188"/>
+      <c r="I27" s="188"/>
+      <c r="J27" s="188"/>
+      <c r="K27" s="189"/>
     </row>
     <row r="28" spans="1:11" ht="185.25" customHeight="1">
       <c r="A28" s="76">
@@ -5700,17 +5720,17 @@
       <c r="B28" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="180" t="s">
+      <c r="C28" s="187" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="181"/>
-      <c r="E28" s="181"/>
-      <c r="F28" s="181"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="181"/>
-      <c r="I28" s="181"/>
-      <c r="J28" s="181"/>
-      <c r="K28" s="182"/>
+      <c r="D28" s="188"/>
+      <c r="E28" s="188"/>
+      <c r="F28" s="188"/>
+      <c r="G28" s="188"/>
+      <c r="H28" s="188"/>
+      <c r="I28" s="188"/>
+      <c r="J28" s="188"/>
+      <c r="K28" s="189"/>
     </row>
     <row r="29" spans="1:11" ht="156.75" customHeight="1">
       <c r="A29" s="76">
@@ -5719,17 +5739,17 @@
       <c r="B29" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="180" t="s">
+      <c r="C29" s="187" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="181"/>
-      <c r="E29" s="181"/>
-      <c r="F29" s="181"/>
-      <c r="G29" s="181"/>
-      <c r="H29" s="181"/>
-      <c r="I29" s="181"/>
-      <c r="J29" s="181"/>
-      <c r="K29" s="182"/>
+      <c r="D29" s="188"/>
+      <c r="E29" s="188"/>
+      <c r="F29" s="188"/>
+      <c r="G29" s="188"/>
+      <c r="H29" s="188"/>
+      <c r="I29" s="188"/>
+      <c r="J29" s="188"/>
+      <c r="K29" s="189"/>
     </row>
     <row r="30" spans="1:11" ht="213.75" customHeight="1">
       <c r="A30" s="76">
@@ -5738,17 +5758,17 @@
       <c r="B30" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="180" t="s">
+      <c r="C30" s="187" t="s">
         <v>134</v>
       </c>
-      <c r="D30" s="181"/>
-      <c r="E30" s="181"/>
-      <c r="F30" s="181"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="181"/>
-      <c r="I30" s="181"/>
-      <c r="J30" s="181"/>
-      <c r="K30" s="182"/>
+      <c r="D30" s="188"/>
+      <c r="E30" s="188"/>
+      <c r="F30" s="188"/>
+      <c r="G30" s="188"/>
+      <c r="H30" s="188"/>
+      <c r="I30" s="188"/>
+      <c r="J30" s="188"/>
+      <c r="K30" s="189"/>
     </row>
     <row r="31" spans="1:11" ht="114" customHeight="1">
       <c r="A31" s="76">
@@ -5757,17 +5777,17 @@
       <c r="B31" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="180" t="s">
+      <c r="C31" s="187" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
+      <c r="D31" s="188"/>
+      <c r="E31" s="188"/>
+      <c r="F31" s="188"/>
+      <c r="G31" s="188"/>
+      <c r="H31" s="188"/>
+      <c r="I31" s="188"/>
+      <c r="J31" s="188"/>
+      <c r="K31" s="189"/>
     </row>
     <row r="32" spans="1:11" ht="99.75" customHeight="1">
       <c r="A32" s="76">
@@ -5776,17 +5796,17 @@
       <c r="B32" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="180" t="s">
+      <c r="C32" s="187" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="181"/>
-      <c r="E32" s="181"/>
-      <c r="F32" s="181"/>
-      <c r="G32" s="181"/>
-      <c r="H32" s="181"/>
-      <c r="I32" s="181"/>
-      <c r="J32" s="181"/>
-      <c r="K32" s="182"/>
+      <c r="D32" s="188"/>
+      <c r="E32" s="188"/>
+      <c r="F32" s="188"/>
+      <c r="G32" s="188"/>
+      <c r="H32" s="188"/>
+      <c r="I32" s="188"/>
+      <c r="J32" s="188"/>
+      <c r="K32" s="189"/>
     </row>
     <row r="33" spans="1:11" ht="171" customHeight="1">
       <c r="A33" s="76">
@@ -5795,17 +5815,17 @@
       <c r="B33" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="180" t="s">
+      <c r="C33" s="187" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="181"/>
-      <c r="E33" s="181"/>
-      <c r="F33" s="181"/>
-      <c r="G33" s="181"/>
-      <c r="H33" s="181"/>
-      <c r="I33" s="181"/>
-      <c r="J33" s="181"/>
-      <c r="K33" s="182"/>
+      <c r="D33" s="188"/>
+      <c r="E33" s="188"/>
+      <c r="F33" s="188"/>
+      <c r="G33" s="188"/>
+      <c r="H33" s="188"/>
+      <c r="I33" s="188"/>
+      <c r="J33" s="188"/>
+      <c r="K33" s="189"/>
     </row>
     <row r="34" spans="1:11" ht="171" customHeight="1">
       <c r="A34" s="76">
@@ -5814,17 +5834,17 @@
       <c r="B34" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="C34" s="180" t="s">
+      <c r="C34" s="187" t="s">
         <v>142</v>
       </c>
-      <c r="D34" s="181"/>
-      <c r="E34" s="181"/>
-      <c r="F34" s="181"/>
-      <c r="G34" s="181"/>
-      <c r="H34" s="181"/>
-      <c r="I34" s="181"/>
-      <c r="J34" s="181"/>
-      <c r="K34" s="182"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188"/>
+      <c r="F34" s="188"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="188"/>
+      <c r="I34" s="188"/>
+      <c r="J34" s="188"/>
+      <c r="K34" s="189"/>
     </row>
     <row r="35" spans="1:11" ht="111.75" customHeight="1" thickBot="1">
       <c r="A35" s="77">
@@ -5833,17 +5853,17 @@
       <c r="B35" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="183" t="s">
+      <c r="C35" s="190" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="184"/>
-      <c r="E35" s="184"/>
-      <c r="F35" s="184"/>
-      <c r="G35" s="184"/>
-      <c r="H35" s="184"/>
-      <c r="I35" s="184"/>
-      <c r="J35" s="184"/>
-      <c r="K35" s="185"/>
+      <c r="D35" s="191"/>
+      <c r="E35" s="191"/>
+      <c r="F35" s="191"/>
+      <c r="G35" s="191"/>
+      <c r="H35" s="191"/>
+      <c r="I35" s="191"/>
+      <c r="J35" s="191"/>
+      <c r="K35" s="192"/>
     </row>
     <row r="36" spans="1:11" ht="15" thickTop="1"/>
   </sheetData>
@@ -5872,7 +5892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="C44" sqref="C44:C48"/>
     </sheetView>
   </sheetViews>
@@ -5884,12 +5904,12 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A2" s="27"/>
-      <c r="B2" s="188" t="s">
+      <c r="B2" s="195" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -6326,7 +6346,7 @@
   <dimension ref="A2:O18"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6342,22 +6362,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="48.75" customHeight="1" thickBot="1">
-      <c r="B2" s="190" t="s">
+      <c r="B2" s="197" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-      <c r="K2" s="191"/>
-      <c r="L2" s="191"/>
-      <c r="M2" s="191"/>
-      <c r="N2" s="191"/>
-      <c r="O2" s="191"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="198"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickTop="1"/>
     <row r="4" spans="1:15" ht="36" customHeight="1">
@@ -6391,18 +6411,18 @@
       <c r="D5" s="64"/>
       <c r="E5" s="64">
         <f>SUM(E7:E15)</f>
-        <v>13.5</v>
+        <v>4.5</v>
       </c>
       <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:15" ht="18.75">
       <c r="A6" s="67"/>
-      <c r="B6" s="193" t="s">
+      <c r="B6" s="118" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="194"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="194"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
       <c r="F6" s="85"/>
       <c r="H6" s="23" t="s">
         <v>217</v>
@@ -6462,15 +6482,15 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="64">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="64">
         <f t="shared" ref="E8:E15" si="0" xml:space="preserve"> C8 * D8</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="48">
         <f t="shared" ref="F8:F15" si="1">IF(E8&lt;=0,0,IF(E8&lt;=1,0.05,IF(E8&lt;=2,0.1,IF(E8&lt;=3,0.6,1))))</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H8" s="39" t="s">
         <v>208</v>
@@ -6496,15 +6516,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="64">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="64">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="48">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="39" t="s">
         <v>209</v>
@@ -6558,15 +6578,15 @@
         <v>1</v>
       </c>
       <c r="D11" s="64">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="64">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F11" s="48">
         <f>IF(E11&lt;=0,0,IF(E11&lt;=1,0.05,IF(E11&lt;=2,0.1,IF(E11&lt;=3,0.6,1))))</f>
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H11" s="87" t="s">
         <v>211</v>
@@ -6577,12 +6597,12 @@
     </row>
     <row r="12" spans="1:15" ht="15" thickTop="1">
       <c r="A12" s="67"/>
-      <c r="B12" s="193" t="s">
+      <c r="B12" s="118" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="194"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
       <c r="F12" s="85"/>
     </row>
     <row r="13" spans="1:15">
@@ -6665,7 +6685,7 @@
       <c r="E16" s="64"/>
       <c r="F16" s="95">
         <f>SUM(F7:F15)</f>
-        <v>4.1500000000000004</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I16" s="97"/>
     </row>
@@ -6681,7 +6701,7 @@
       <c r="E17" s="94"/>
       <c r="F17" s="96">
         <f>IF(F16&lt;1,48,IF(F16&lt;3,32,20))</f>
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickTop="1">

</xml_diff>